<commit_message>
Add histogram for grades
</commit_message>
<xml_diff>
--- a/Test/testdata.xlsx
+++ b/Test/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aufgabe 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabe 7</t>
   </si>
   <si>
     <t>Gesamt</t>
@@ -675,10 +678,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -698,10 +704,13 @@
       <c r="G2">
         <v>10</v>
       </c>
+      <c r="H2" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -721,10 +730,13 @@
       <c r="G3">
         <v>8</v>
       </c>
+      <c r="H3" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -742,12 +754,15 @@
         <v>5</v>
       </c>
       <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -767,10 +782,13 @@
       <c r="G5">
         <v>10</v>
       </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -788,12 +806,15 @@
         <v>4</v>
       </c>
       <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -811,12 +832,15 @@
         <v>5</v>
       </c>
       <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -834,12 +858,15 @@
         <v>2</v>
       </c>
       <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -857,12 +884,15 @@
         <v>1</v>
       </c>
       <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -880,12 +910,15 @@
         <v>1</v>
       </c>
       <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
@@ -905,10 +938,13 @@
       <c r="G11" s="2">
         <v>10</v>
       </c>
+      <c r="H11" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
@@ -928,10 +964,13 @@
       <c r="G12" s="2">
         <v>8</v>
       </c>
+      <c r="H12" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>2</v>
@@ -951,10 +990,13 @@
       <c r="G13" s="2">
         <v>2</v>
       </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>3</v>
@@ -974,10 +1016,13 @@
       <c r="G14" s="2">
         <v>10</v>
       </c>
+      <c r="H14" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -995,12 +1040,15 @@
         <v>4</v>
       </c>
       <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -1020,10 +1068,13 @@
       <c r="G16" s="2">
         <v>5</v>
       </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -1043,10 +1094,13 @@
       <c r="G17" s="2">
         <v>8</v>
       </c>
+      <c r="H17" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
         <v>2</v>
@@ -1064,12 +1118,15 @@
         <v>1</v>
       </c>
       <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
         <v>3</v>
@@ -1089,10 +1146,13 @@
       <c r="G19" s="2">
         <v>10</v>
       </c>
+      <c r="H19" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
@@ -1110,12 +1170,15 @@
         <v>4</v>
       </c>
       <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
@@ -1133,12 +1196,15 @@
         <v>5</v>
       </c>
       <c r="G21" s="2">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2">
         <v>2</v>
@@ -1156,12 +1222,15 @@
         <v>4</v>
       </c>
       <c r="G22" s="2">
+        <v>3</v>
+      </c>
+      <c r="H22" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
@@ -1179,12 +1248,15 @@
         <v>1</v>
       </c>
       <c r="G23" s="2">
+        <v>3</v>
+      </c>
+      <c r="H23" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
@@ -1202,12 +1274,15 @@
         <v>4</v>
       </c>
       <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
@@ -1225,6 +1300,9 @@
         <v>4</v>
       </c>
       <c r="G25" s="2">
+        <v>10</v>
+      </c>
+      <c r="H25" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>